<commit_message>
ETF and indices selected roughly.
</commit_message>
<xml_diff>
--- a/0.Data/ETF List.xlsx
+++ b/0.Data/ETF List.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_AD4DC2C4214B839BC62F9C83E64E2CC26AE8DE2C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1BCC824C-EDBD-407D-A035-596E886EFA06}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_AD4DC2C4214B839BC62F9C83E64E2CC26AE8DE2C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{DF0B252A-1D14-477A-9CF8-B2F69548A59E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$644</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="607">
   <si>
     <t>ACWI - iShares MSCI ACWI Index Fund </t>
   </si>
@@ -1802,6 +1805,58 @@
   </si>
   <si>
     <t>AAXJ - iShares MSCI All Country Asia ex Japan Index Fund </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>volumn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>volatility</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>option volumn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YYY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>^GSPC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>^RUT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>^VIX</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2143,3151 +2198,3390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A643"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E647"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D649" sqref="D649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D1" t="s">
+        <v>599</v>
+      </c>
+      <c r="E1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C3">
+        <v>2482800</v>
+      </c>
+      <c r="E3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C6">
+        <v>17900</v>
+      </c>
+      <c r="E6" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>595</v>
+      </c>
+      <c r="C7">
+        <v>2413900</v>
+      </c>
+      <c r="E7" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B13" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>601</v>
+      </c>
+      <c r="C28">
+        <v>1917900</v>
+      </c>
+      <c r="E28" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+      <c r="B77" t="s">
+        <v>601</v>
+      </c>
+      <c r="C77">
+        <v>1027400</v>
+      </c>
+      <c r="E77" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="1"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
+    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
+    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
+    <row r="145" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
+    <row r="146" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
+    <row r="147" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
+    <row r="148" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
+    <row r="149" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" s="1" t="s">
+    <row r="150" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
+    <row r="153" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153" s="1" t="s">
+    <row r="154" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
+    <row r="155" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
+    <row r="156" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
+    <row r="157" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157" s="1" t="s">
+    <row r="158" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158" s="1" t="s">
+    <row r="159" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159" s="1" t="s">
+    <row r="160" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
+    <row r="161" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="1" t="s">
+    <row r="162" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="1" t="s">
+    <row r="163" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
+    <row r="164" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="1" t="s">
+    <row r="165" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167" s="1" t="s">
+    <row r="168" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
+    <row r="169" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169" s="1" t="s">
+    <row r="170" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
+    <row r="171" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+    <row r="172" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" s="1" t="s">
+    <row r="173" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" s="1" t="s">
+    <row r="174" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174" s="1" t="s">
+    <row r="175" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
+    <row r="176" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" s="1" t="s">
+    <row r="177" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
+    <row r="178" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179" s="1" t="s">
+    <row r="179" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" s="1" t="s">
+    <row r="181" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181" s="1" t="s">
+    <row r="182" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A182" s="1" t="s">
+    <row r="183" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A183" s="1" t="s">
+    <row r="184" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A184" s="1" t="s">
+    <row r="185" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A185" s="1" t="s">
+    <row r="186" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A186" s="1" t="s">
+    <row r="187" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187" s="1" t="s">
+    <row r="188" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A188" s="1" t="s">
+    <row r="189" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A189" s="1" t="s">
+    <row r="190" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A190" s="1" t="s">
+    <row r="191" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A192" s="1" t="s">
+    <row r="192" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A193" s="1" t="s">
+    <row r="194" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A194" s="1" t="s">
+    <row r="195" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A195" s="1" t="s">
+    <row r="196" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196" s="1" t="s">
+    <row r="197" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A197" s="1" t="s">
+    <row r="198" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A198" s="1" t="s">
+    <row r="199" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A199" s="1" t="s">
+    <row r="200" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200" s="1" t="s">
+    <row r="201" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A201" s="1" t="s">
+    <row r="202" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A202" s="1" t="s">
+    <row r="203" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" s="1"/>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A204" s="1" t="s">
+    <row r="204" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A205" s="1" t="s">
+    <row r="206" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A206" s="1" t="s">
+    <row r="207" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A207" s="1" t="s">
+    <row r="208" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A208" s="1" t="s">
+    <row r="209" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A209" s="1" t="s">
+    <row r="210" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A210" s="1" t="s">
+    <row r="211" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A211" s="1" t="s">
+    <row r="212" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A212" s="1" t="s">
+    <row r="213" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" s="1" t="s">
+    <row r="214" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A214" s="1" t="s">
+    <row r="215" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A215" s="1" t="s">
+    <row r="216" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A216" s="1"/>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A217" s="1" t="s">
+    <row r="217" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A218" s="1" t="s">
+    <row r="219" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A219" s="1" t="s">
+    <row r="220" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A220" s="1" t="s">
+    <row r="221" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A221" s="1" t="s">
+    <row r="222" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A222" s="1" t="s">
+    <row r="223" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A223" s="1" t="s">
+    <row r="224" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A224" s="1" t="s">
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A225" s="1" t="s">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A226" s="1" t="s">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A227" s="1"/>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A228" s="1" t="s">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A230" s="1" t="s">
+    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A231" s="1" t="s">
+    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A232" s="1" t="s">
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A233" s="1" t="s">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A234" s="1" t="s">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A235" s="1" t="s">
+      <c r="B235" t="s">
+        <v>601</v>
+      </c>
+      <c r="C235">
+        <v>89300</v>
+      </c>
+      <c r="E235" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A236" s="1" t="s">
+    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A237" s="1" t="s">
+    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A238" s="1" t="s">
+    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A239" s="1" t="s">
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A240" s="1"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A241" s="1" t="s">
+    <row r="241" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A242" s="1" t="s">
+    <row r="243" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A243" s="1" t="s">
+    <row r="244" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A244" s="1" t="s">
+    <row r="245" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A245" s="1" t="s">
+    <row r="246" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A246" s="1" t="s">
+    <row r="247" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A247" s="1" t="s">
+    <row r="248" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A248" s="1" t="s">
+    <row r="249" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A249" s="1" t="s">
+    <row r="250" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A250" s="1" t="s">
+    <row r="251" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A251" s="1" t="s">
+    <row r="252" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A252" s="1" t="s">
+    <row r="253" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A253" s="1"/>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A254" s="1" t="s">
+    <row r="254" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="1"/>
+    </row>
+    <row r="255" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A255" s="1" t="s">
+    <row r="256" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A256" s="1" t="s">
+    <row r="257" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A257" s="1" t="s">
+    <row r="258" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A258" s="1" t="s">
+    <row r="259" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A259" s="1" t="s">
+    <row r="260" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A260" s="1" t="s">
+    <row r="261" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A261" s="1" t="s">
+    <row r="262" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A262" s="1" t="s">
+    <row r="263" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A263" s="1" t="s">
+    <row r="264" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A264" s="1" t="s">
+    <row r="265" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A265" s="1"/>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A266" s="1" t="s">
+    <row r="266" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="1"/>
+    </row>
+    <row r="267" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A267" s="1" t="s">
+    <row r="268" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A268" s="1" t="s">
+    <row r="269" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A269" s="1" t="s">
+    <row r="270" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A270" s="1" t="s">
+    <row r="271" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A271" s="1" t="s">
+    <row r="272" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A272" s="1" t="s">
+    <row r="273" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A273" s="1" t="s">
+    <row r="274" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A274" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A274" s="1" t="s">
+    <row r="275" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A275" s="1" t="s">
+    <row r="276" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A276" s="1" t="s">
+    <row r="277" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A277" s="1"/>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A278" s="1" t="s">
+    <row r="278" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="1"/>
+    </row>
+    <row r="279" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A279" s="1" t="s">
+    <row r="280" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A280" s="1" t="s">
+    <row r="281" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A281" s="1" t="s">
+    <row r="282" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A282" s="1" t="s">
+    <row r="283" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A283" s="1" t="s">
+    <row r="284" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A284" s="1" t="s">
+    <row r="285" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A285" s="1" t="s">
+    <row r="286" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A286" s="1" t="s">
+    <row r="287" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A287" s="1" t="s">
+    <row r="288" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A288" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A288" s="1"/>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A289" s="1" t="s">
+    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="1"/>
+    </row>
+    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A290" s="1" t="s">
+    <row r="291" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A291" s="1" t="s">
+    <row r="292" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A292" s="1" t="s">
+    <row r="293" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A293" s="1" t="s">
+    <row r="294" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A294" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A294" s="1" t="s">
+    <row r="295" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A295" s="1" t="s">
+    <row r="296" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A296" s="1" t="s">
+    <row r="297" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A297" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A297" s="1" t="s">
+    <row r="298" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A298" s="1" t="s">
+    <row r="299" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A299" s="1" t="s">
+    <row r="300" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A300" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A300" s="1" t="s">
+    <row r="301" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A301" s="1"/>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A302" s="1" t="s">
+    <row r="302" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A302" s="1"/>
+    </row>
+    <row r="303" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A303" s="1" t="s">
+    <row r="304" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A304" s="1" t="s">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A305" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A305" s="1" t="s">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A306" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A306" s="1" t="s">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A307" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A307" s="1" t="s">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A308" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A308" s="1" t="s">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A309" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A309" s="1" t="s">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A310" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A310" s="1" t="s">
+      <c r="B310" t="s">
+        <v>601</v>
+      </c>
+      <c r="C310">
+        <v>4832800</v>
+      </c>
+      <c r="E310" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A311" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A311" s="1" t="s">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A312" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A312" s="1" t="s">
+      <c r="B312" t="s">
+        <v>601</v>
+      </c>
+      <c r="C312">
+        <v>715700</v>
+      </c>
+      <c r="E312" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A313" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A313" s="1" t="s">
+    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A314" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A314" s="1" t="s">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A315" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A315" s="1"/>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A316" s="1" t="s">
+    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="1"/>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A317" s="1" t="s">
+      <c r="B317" t="s">
+        <v>601</v>
+      </c>
+      <c r="C317">
+        <v>26409500</v>
+      </c>
+      <c r="E317" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A318" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A318" s="1" t="s">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A319" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A319" s="1" t="s">
+    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A320" s="1" t="s">
+    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A321" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A321" s="1" t="s">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A322" s="1" t="s">
+    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A323" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A323" s="1" t="s">
+      <c r="B323" t="s">
+        <v>601</v>
+      </c>
+      <c r="C323">
+        <v>195700</v>
+      </c>
+      <c r="E323" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A324" s="1" t="s">
+    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A325" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A325" s="1" t="s">
+    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A326" s="1" t="s">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A327" s="1" t="s">
+    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A328" s="1"/>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A329" s="1" t="s">
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="1"/>
+    </row>
+    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A330" s="1" t="s">
+    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A331" s="1" t="s">
+    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A332" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A332" s="1" t="s">
+    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A333" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A333" s="1" t="s">
+    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A334" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A334" s="1" t="s">
+    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A335" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A335" s="1" t="s">
+    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A336" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A336" s="1" t="s">
+    <row r="337" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A337" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A337" s="1" t="s">
+    <row r="338" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A338" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A338" s="1" t="s">
+    <row r="339" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A339" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A339" s="1"/>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A340" s="1" t="s">
+    <row r="340" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A340" s="1"/>
+    </row>
+    <row r="341" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A341" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A341" s="1" t="s">
+    <row r="342" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A342" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A342" s="1" t="s">
+    <row r="343" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A343" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A343" s="1" t="s">
+    <row r="344" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A344" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A344" s="1" t="s">
+    <row r="345" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A345" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A345" s="1" t="s">
+    <row r="346" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A346" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A346" s="1" t="s">
+    <row r="347" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A347" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A347" s="1" t="s">
+    <row r="348" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A348" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A348" s="1" t="s">
+    <row r="349" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A349" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A349" s="1" t="s">
+    <row r="350" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A350" s="1" t="s">
+    <row r="351" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A351" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A351" s="1"/>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A352" s="1" t="s">
+    <row r="352" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="1"/>
+    </row>
+    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A353" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A353" s="1" t="s">
+    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A354" s="1" t="s">
+    <row r="355" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A355" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A355" s="1" t="s">
+    <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A356" s="1" t="s">
+    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A357" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A357" s="1" t="s">
+    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A358" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A358" s="1" t="s">
+    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A359" s="1" t="s">
+    <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A360" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A360" s="1" t="s">
+    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A361" s="1" t="s">
+    <row r="362" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A362" s="1" t="s">
+    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A363" s="1" t="s">
+    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A364" s="1"/>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A365" s="1" t="s">
+    <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="1"/>
+    </row>
+    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A366" s="1" t="s">
+    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A367" s="1" t="s">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A368" s="1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A368" s="1" t="s">
+      <c r="B368" t="s">
+        <v>601</v>
+      </c>
+      <c r="C368">
+        <v>4872900</v>
+      </c>
+      <c r="E368" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A369" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A369" s="1" t="s">
+    <row r="370" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A370" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A370" s="1" t="s">
+    <row r="371" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A371" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A371" s="1" t="s">
+    <row r="372" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A372" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A372" s="1" t="s">
+    <row r="373" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A373" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A373" s="1" t="s">
+    <row r="374" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A374" s="1" t="s">
+    <row r="375" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A375" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A375" s="1" t="s">
+    <row r="376" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A376" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A376" s="1" t="s">
+    <row r="377" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A377" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A377" s="1"/>
-    </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A378" s="1" t="s">
+    <row r="378" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A378" s="1"/>
+    </row>
+    <row r="379" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A379" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A379" s="1" t="s">
+    <row r="380" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A380" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A380" s="1" t="s">
+    <row r="381" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A381" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A381" s="1" t="s">
+    <row r="382" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A382" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A382" s="1" t="s">
+    <row r="383" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A383" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A383" s="1" t="s">
+    <row r="384" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A384" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A384" s="1" t="s">
+    <row r="385" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A385" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A385" s="1" t="s">
+    <row r="386" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A386" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A386" s="1" t="s">
+    <row r="387" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A387" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A387" s="1" t="s">
+    <row r="388" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A388" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A388" s="1" t="s">
+    <row r="389" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A389" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A389" s="1"/>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A390" s="1" t="s">
+    <row r="390" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A390" s="1"/>
+    </row>
+    <row r="391" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A391" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A391" s="1" t="s">
+    <row r="392" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A392" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A392" s="1" t="s">
+    <row r="393" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A393" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A393" s="1" t="s">
+    <row r="394" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A394" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A394" s="1" t="s">
+    <row r="395" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A395" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A395" s="1" t="s">
+    <row r="396" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A396" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A396" s="1" t="s">
+    <row r="397" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A397" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A397" s="1" t="s">
+    <row r="398" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A398" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A398" s="1" t="s">
+    <row r="399" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A399" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A399" s="1" t="s">
+    <row r="400" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A400" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A400" s="1" t="s">
+    <row r="401" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A401" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A401" s="1"/>
-    </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A402" s="1" t="s">
+    <row r="402" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A402" s="1"/>
+    </row>
+    <row r="403" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A403" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A403" s="1" t="s">
+    <row r="404" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A404" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A404" s="1" t="s">
+    <row r="405" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A405" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A405" s="1" t="s">
+    <row r="406" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A406" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A406" s="1" t="s">
+    <row r="407" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A407" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A407" s="1" t="s">
+    <row r="408" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A408" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A408" s="1" t="s">
+    <row r="409" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A409" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A409" s="1" t="s">
+    <row r="410" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A410" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A410" s="1" t="s">
+    <row r="411" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A411" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A411" s="1" t="s">
+    <row r="412" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A412" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A412" s="1"/>
-    </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A413" s="1" t="s">
+    <row r="413" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A413" s="1"/>
+    </row>
+    <row r="414" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A414" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A414" s="1" t="s">
+    <row r="415" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A415" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A415" s="1" t="s">
+    <row r="416" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A416" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A416" s="1" t="s">
+    <row r="417" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A417" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A417" s="1" t="s">
+    <row r="418" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A418" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A418" s="1" t="s">
+    <row r="419" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A419" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A419" s="1" t="s">
+    <row r="420" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A420" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A420" s="1" t="s">
+    <row r="421" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A421" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A421" s="1" t="s">
+    <row r="422" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A422" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A422" s="1" t="s">
+    <row r="423" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A423" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A423" s="1" t="s">
+    <row r="424" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A424" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A424" s="1"/>
-    </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A425" s="1" t="s">
+    <row r="425" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A425" s="1"/>
+    </row>
+    <row r="426" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A426" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A426" s="1" t="s">
+    <row r="427" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A427" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A427" s="1" t="s">
+    <row r="428" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A428" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A428" s="1" t="s">
+    <row r="429" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A429" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A429" s="1" t="s">
+    <row r="430" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A430" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A430" s="1" t="s">
+    <row r="431" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A431" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A431" s="1" t="s">
+    <row r="432" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A432" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A432" s="1" t="s">
+    <row r="433" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A433" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A433" s="1" t="s">
+    <row r="434" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A434" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A434" s="1" t="s">
+    <row r="435" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A435" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A435" s="1" t="s">
+    <row r="436" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A436" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A436" s="1" t="s">
+    <row r="437" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A437" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A437" s="1"/>
-    </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A438" s="1" t="s">
+    <row r="438" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A438" s="1"/>
+    </row>
+    <row r="439" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A439" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A439" s="1" t="s">
+    <row r="440" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A440" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A440" s="1" t="s">
+    <row r="441" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A441" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A441" s="1" t="s">
+    <row r="442" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A442" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A442" s="1" t="s">
+    <row r="443" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A443" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A443" s="1" t="s">
+    <row r="444" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A444" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A444" s="1" t="s">
+    <row r="445" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A445" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A445" s="1" t="s">
+    <row r="446" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A446" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A446" s="1" t="s">
+    <row r="447" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A447" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A447" s="1" t="s">
+    <row r="448" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A448" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A448" s="1" t="s">
+    <row r="449" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A449" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A449" s="1" t="s">
+    <row r="450" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A450" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A450" s="1" t="s">
+    <row r="451" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A451" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A451" s="1"/>
-    </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A452" s="1" t="s">
+    <row r="452" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A452" s="1"/>
+    </row>
+    <row r="453" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A453" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A453" s="1" t="s">
+    <row r="454" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A454" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A454" s="1" t="s">
+    <row r="455" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A455" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A455" s="1" t="s">
+    <row r="456" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A456" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A456" s="1" t="s">
+    <row r="457" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A457" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A457" s="1" t="s">
+    <row r="458" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A458" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A458" s="1" t="s">
+    <row r="459" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A459" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A459" s="1" t="s">
+    <row r="460" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A460" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A460" s="1" t="s">
+    <row r="461" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A461" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A461" s="1" t="s">
+    <row r="462" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A462" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A462" s="1" t="s">
+    <row r="463" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A463" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A463" s="1" t="s">
+    <row r="464" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A464" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A464" s="1" t="s">
+    <row r="465" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A465" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A465" s="1" t="s">
+    <row r="466" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A466" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A466" s="1"/>
-    </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A467" s="1" t="s">
+    <row r="467" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A467" s="1"/>
+    </row>
+    <row r="468" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A468" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A468" s="1" t="s">
+    <row r="469" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A469" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A469" s="1" t="s">
+    <row r="470" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A470" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A470" s="1" t="s">
+    <row r="471" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A471" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A471" s="1" t="s">
+    <row r="472" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A472" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A472" s="1" t="s">
+    <row r="473" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A473" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A473" s="1" t="s">
+    <row r="474" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A474" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A474" s="1" t="s">
+    <row r="475" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A475" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A475" s="1" t="s">
+    <row r="476" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A476" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A476" s="1" t="s">
+    <row r="477" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A477" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A477" s="1" t="s">
+    <row r="478" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A478" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A478" s="1" t="s">
+    <row r="479" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A479" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A479" s="1" t="s">
+    <row r="480" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A480" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A480" s="1"/>
-    </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A481" s="1" t="s">
+    <row r="481" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A481" s="1"/>
+    </row>
+    <row r="482" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A482" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A482" s="1" t="s">
+    <row r="483" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A483" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A483" s="1" t="s">
+    <row r="484" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A484" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A484" s="1" t="s">
+    <row r="485" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A485" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A485" s="1" t="s">
+    <row r="486" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A486" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A486" s="1" t="s">
+    <row r="487" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A487" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A487" s="1" t="s">
+    <row r="488" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A488" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A488" s="1" t="s">
+    <row r="489" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A489" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A489" s="1" t="s">
+    <row r="490" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A490" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A490" s="1" t="s">
+    <row r="491" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A491" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A491" s="1" t="s">
+    <row r="492" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A492" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A492" s="1" t="s">
+    <row r="493" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A493" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A493" s="1" t="s">
+    <row r="494" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A494" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A494" s="1" t="s">
+    <row r="495" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A495" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A495" s="1"/>
-    </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A496" s="1" t="s">
+    <row r="496" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A496" s="1"/>
+    </row>
+    <row r="497" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A497" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A497" s="1" t="s">
+    <row r="498" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A498" s="1" t="s">
+    <row r="499" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A499" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A499" s="1" t="s">
+    <row r="500" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A500" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A500" s="1" t="s">
+    <row r="501" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A501" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A501" s="1" t="s">
+    <row r="502" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A502" s="1" t="s">
+    <row r="503" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A503" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A503" s="1" t="s">
+    <row r="504" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A504" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A504" s="1" t="s">
+    <row r="505" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A505" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A505" s="1" t="s">
+    <row r="506" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A506" s="1" t="s">
+    <row r="507" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A507" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A507" s="1" t="s">
+    <row r="508" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A508" s="1" t="s">
+    <row r="509" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A509" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A509" s="1"/>
-    </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A510" s="1" t="s">
+    <row r="510" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A510" s="1"/>
+    </row>
+    <row r="511" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A511" s="1" t="s">
+    <row r="512" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A512" s="1" t="s">
+    <row r="513" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A513" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A513" s="1" t="s">
+    <row r="514" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A514" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A514" s="1" t="s">
+    <row r="515" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A515" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A515" s="1" t="s">
+    <row r="516" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A516" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A516" s="1" t="s">
+    <row r="517" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A517" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A517" s="1" t="s">
+    <row r="518" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A518" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A518" s="1" t="s">
+    <row r="519" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A519" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A519" s="1" t="s">
+    <row r="520" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A520" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A520" s="1" t="s">
+    <row r="521" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A521" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A521" s="1" t="s">
+    <row r="522" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A522" s="1" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A522" s="1" t="s">
+    <row r="523" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A523" s="1" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A523" s="1"/>
-    </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A524" s="1" t="s">
+    <row r="524" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A524" s="1"/>
+    </row>
+    <row r="525" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A525" s="1" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A525" s="1" t="s">
+    <row r="526" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A526" s="1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A526" s="1" t="s">
+    <row r="527" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A527" s="1" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A527" s="1" t="s">
+    <row r="528" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A528" s="1" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A528" s="1" t="s">
+    <row r="529" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A529" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A529" s="1" t="s">
+    <row r="530" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A530" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A530" s="1" t="s">
+    <row r="531" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A531" s="1" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A531" s="1" t="s">
+    <row r="532" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A532" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A532" s="1" t="s">
+    <row r="533" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A533" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A533" s="1" t="s">
+    <row r="534" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A534" s="1" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A534" s="1"/>
-    </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A535" s="1" t="s">
+    <row r="535" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A535" s="1"/>
+    </row>
+    <row r="536" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A536" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A536" s="1" t="s">
+    <row r="537" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A537" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A537" s="1" t="s">
+    <row r="538" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A538" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A538" s="1" t="s">
+    <row r="539" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A539" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A539" s="1" t="s">
+    <row r="540" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A540" s="1" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A540" s="1" t="s">
+    <row r="541" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A541" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A541" s="1" t="s">
+    <row r="542" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A542" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A542" s="1" t="s">
+    <row r="543" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A543" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A543" s="1" t="s">
+    <row r="544" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A544" s="1" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A544" s="1" t="s">
+    <row r="545" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A545" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A545" s="1" t="s">
+    <row r="546" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A546" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A546" s="1"/>
-    </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A547" s="1" t="s">
+    <row r="547" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A547" s="1"/>
+    </row>
+    <row r="548" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A548" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A548" s="1" t="s">
+    <row r="549" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A549" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A549" s="1" t="s">
+    <row r="550" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A550" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A550" s="1" t="s">
+    <row r="551" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A551" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A551" s="1" t="s">
+      <c r="B551" t="s">
+        <v>601</v>
+      </c>
+      <c r="C551">
+        <v>50100</v>
+      </c>
+      <c r="E551" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A552" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A552" s="1" t="s">
+    <row r="553" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A553" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A553" s="1" t="s">
+    <row r="554" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A554" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A554" s="1" t="s">
+    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A555" s="1" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A555" s="1" t="s">
+      <c r="B555" t="s">
+        <v>601</v>
+      </c>
+      <c r="C555">
+        <v>4433600</v>
+      </c>
+      <c r="E555" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A556" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A556" s="1" t="s">
+    <row r="557" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A557" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A557" s="1" t="s">
+    <row r="558" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A558" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="558" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A558" s="1" t="s">
+    <row r="559" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A559" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A559" s="1" t="s">
+    <row r="560" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A560" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A560" s="1"/>
-    </row>
-    <row r="561" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A561" s="1" t="s">
+    <row r="561" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A561" s="1"/>
+    </row>
+    <row r="562" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A562" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="562" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A562" s="1" t="s">
+    <row r="563" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A563" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="563" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A563" s="1" t="s">
+    <row r="564" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A564" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="564" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A564" s="1" t="s">
+    <row r="565" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A565" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="565" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A565" s="1" t="s">
+    <row r="566" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A566" s="1" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="566" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A566" s="1" t="s">
+    <row r="567" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A567" s="1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="567" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A567" s="1" t="s">
+    <row r="568" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A568" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="568" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A568" s="1" t="s">
+    <row r="569" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A569" s="1" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="569" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A569" s="1" t="s">
+    <row r="570" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A570" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="570" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A570" s="1" t="s">
+    <row r="571" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A571" s="1" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="571" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A571" s="1" t="s">
+    <row r="572" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A572" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="572" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A572" s="1" t="s">
+    <row r="573" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A573" s="1" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="573" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A573" s="1" t="s">
+    <row r="574" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A574" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="574" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A574" s="1" t="s">
+    <row r="575" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A575" s="1" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="575" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A575" s="1"/>
-    </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A576" s="1" t="s">
+    <row r="576" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A576" s="1"/>
+    </row>
+    <row r="577" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A577" s="1" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="577" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A577" s="1" t="s">
+    <row r="578" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A578" s="1" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="578" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A578" s="1" t="s">
+    <row r="579" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A579" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="579" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A579" s="1" t="s">
+    <row r="580" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A580" s="1" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="580" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A580" s="1" t="s">
+    <row r="581" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A581" s="1" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="581" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A581" s="1" t="s">
+    <row r="582" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A582" s="1" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="582" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A582" s="1" t="s">
+    <row r="583" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A583" s="1" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="583" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A583" s="1" t="s">
+    <row r="584" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A584" s="1" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="584" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A584" s="1" t="s">
+    <row r="585" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A585" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="585" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A585" s="1" t="s">
+    <row r="586" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A586" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="586" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A586" s="1" t="s">
+    <row r="587" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A587" s="1" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="587" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A587" s="1" t="s">
+    <row r="588" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A588" s="1" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="588" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A588" s="1" t="s">
+    <row r="589" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A589" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="589" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A589" s="1" t="s">
+    <row r="590" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A590" s="1" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="590" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A590" s="1"/>
-    </row>
-    <row r="591" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A591" s="1" t="s">
+    <row r="591" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A591" s="1"/>
+    </row>
+    <row r="592" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A592" s="1" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="592" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A592" s="1" t="s">
+    <row r="593" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A593" s="1" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="593" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A593" s="1" t="s">
+    <row r="594" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A594" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="594" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A594" s="1" t="s">
+    <row r="595" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A595" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="595" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A595" s="1" t="s">
+    <row r="596" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A596" s="1" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="596" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A596" s="1" t="s">
+      <c r="B596" t="s">
+        <v>601</v>
+      </c>
+      <c r="C596">
+        <v>2804100</v>
+      </c>
+      <c r="E596" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A597" s="1" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="597" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A597" s="1" t="s">
+    <row r="598" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A598" s="1" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="598" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A598" s="1" t="s">
+    <row r="599" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A599" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="599" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A599" s="1" t="s">
+    <row r="600" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A600" s="1" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="600" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A600" s="1" t="s">
+    <row r="601" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A601" s="1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="601" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A601" s="1" t="s">
+    <row r="602" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A602" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="602" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A602" s="1" t="s">
+    <row r="603" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A603" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="603" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A603" s="1" t="s">
+    <row r="604" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A604" s="1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="604" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A604" s="1"/>
-    </row>
-    <row r="605" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A605" s="1" t="s">
+    <row r="605" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A605" s="1"/>
+    </row>
+    <row r="606" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A606" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="606" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A606" s="1" t="s">
+    <row r="607" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A607" s="1" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="607" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A607" s="1" t="s">
+      <c r="B607" t="s">
+        <v>601</v>
+      </c>
+      <c r="C607">
+        <v>88800</v>
+      </c>
+      <c r="E607" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A608" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="608" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A608" s="1" t="s">
+    <row r="609" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A609" s="1" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A609" s="1" t="s">
+    <row r="610" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A610" s="1" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A610" s="1" t="s">
+    <row r="611" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A611" s="1" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A611" s="1" t="s">
+    <row r="612" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A612" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="612" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A612" s="1" t="s">
+    <row r="613" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A613" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="613" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A613" s="1" t="s">
+    <row r="614" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A614" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="614" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A614" s="1" t="s">
+    <row r="615" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A615" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="615" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A615" s="1" t="s">
+    <row r="616" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A616" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="616" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A616" s="1" t="s">
+    <row r="617" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A617" s="1" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="617" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A617" s="1" t="s">
+    <row r="618" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A618" s="1" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="618" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A618" s="1" t="s">
+    <row r="619" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A619" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="619" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A619" s="1"/>
-    </row>
-    <row r="620" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A620" s="1" t="s">
+    <row r="620" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A620" s="1"/>
+    </row>
+    <row r="621" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A621" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="621" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A621" s="1" t="s">
+    <row r="622" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A622" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="622" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A622" s="1" t="s">
+    <row r="623" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A623" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A623" s="1" t="s">
+    <row r="624" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A624" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="624" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A624" s="1" t="s">
+    <row r="625" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A625" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="625" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A625" s="1" t="s">
+    <row r="626" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A626" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="626" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A626" s="1" t="s">
+    <row r="627" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A627" s="1" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="627" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A627" s="1" t="s">
+    <row r="628" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A628" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="628" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A628" s="1" t="s">
+    <row r="629" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A629" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="629" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A629" s="1" t="s">
+    <row r="630" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A630" s="1" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="630" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A630" s="1" t="s">
+    <row r="631" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A631" s="1" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="631" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A631" s="1" t="s">
+      <c r="B631" t="s">
+        <v>601</v>
+      </c>
+      <c r="C631">
+        <v>19100</v>
+      </c>
+      <c r="E631" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A632" s="1" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="632" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A632" s="1" t="s">
+    <row r="633" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A633" s="1" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="633" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A633" s="1" t="s">
+    <row r="634" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A634" s="1" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="634" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A634" s="1"/>
-    </row>
-    <row r="635" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A635" s="1" t="s">
+    <row r="635" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A635" s="1"/>
+    </row>
+    <row r="636" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A636" s="1" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="636" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A636" s="1" t="s">
+    <row r="637" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A637" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="637" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A637" s="1" t="s">
+    <row r="638" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A638" s="1" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="638" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A638" s="1" t="s">
+    <row r="639" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A639" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="639" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A639" s="1" t="s">
+    <row r="640" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A640" s="1" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="640" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A640" s="1" t="s">
+    <row r="641" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A641" s="1" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="641" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A641" s="1" t="s">
+    <row r="642" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A642" s="1" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="642" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A642" s="1" t="s">
+    <row r="643" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A643" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="643" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A643" s="1" t="s">
+    <row r="644" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A644" s="1" t="s">
         <v>592</v>
       </c>
     </row>
+    <row r="645" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A645" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E645" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="646" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A646" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="E646" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="647" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A647" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="E647" t="s">
+        <v>603</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="E1:E644" xr:uid="{021B84DF-B46C-42BE-8F95-15AC20779B95}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Y"/>
+        <filter val="YY"/>
+        <filter val="YYY"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" display="https://www.thebalance.com/list-of-energy-etfs-and-etns-1214760" xr:uid="{11655A6A-FD14-4040-9749-227830CD9695}"/>
-    <hyperlink ref="A20" r:id="rId2" display="https://www.thebalance.com/sdow-a-3x-leveraged-inverse-dow-etf-1215076" xr:uid="{D2112285-2094-4EAA-BE4F-1C95C87AAE55}"/>
-    <hyperlink ref="A22" r:id="rId3" display="https://www.thebalance.com/list-of-leveraged-inverse-etfs-1215227" xr:uid="{9091B37D-4761-448B-BD0A-8BA6049697BA}"/>
-    <hyperlink ref="A34" r:id="rId4" display="https://www.thebalance.com/how-to-invest-in-brazil-with-brazil-etfs-1215127" xr:uid="{7A61D21E-DB11-4DD0-AF99-7D092BB17968}"/>
-    <hyperlink ref="A36" r:id="rId5" display="https://www.thebalance.com/list-of-currency-etfs-and-etns-1215150" xr:uid="{136BEAB0-3B63-402E-90E0-70D6889F7F18}"/>
-    <hyperlink ref="A44" r:id="rId6" display="https://www.thebalance.com/best-cyber-security-etfs-for-2018-4176623" xr:uid="{ABC8736D-C065-4E62-A49B-D9BE59BFAFCD}"/>
-    <hyperlink ref="A48" r:id="rId7" display="https://www.thebalance.com/what-are-futures-and-why-are-they-in-etfs-1214893" xr:uid="{DEC14E35-F05E-43C6-B10B-942E1E443A63}"/>
-    <hyperlink ref="A60" r:id="rId8" display="https://www.thebalance.com/investing-china-etfs-1215166" xr:uid="{9D18CD7A-62E5-4E9C-B26C-E0E802058FB7}"/>
-    <hyperlink ref="A63" r:id="rId9" display="https://www.thebalance.com/learn-the-basics-about-commodity-etfs-1214745" xr:uid="{C7940C82-F295-4443-B03F-6BE2FEFFA78F}"/>
-    <hyperlink ref="A65" r:id="rId10" display="https://www.thebalance.com/gold-etf-what-you-need-to-know-1214748" xr:uid="{7CB792F2-07CC-4BF6-A975-ACDA87540240}"/>
-    <hyperlink ref="A67" r:id="rId11" display="https://www.thebalance.com/how-to-invest-in-oil-without-getting-your-hands-dirty-1214929" xr:uid="{A4BA6A25-556A-4296-941B-A46F8C7D7B8D}"/>
-    <hyperlink ref="A71" r:id="rId12" display="https://www.thebalance.com/list-of-major-oil-etfs-and-etns-1214764" xr:uid="{0130E49E-7202-4A1E-9D26-E5E2E984A789}"/>
-    <hyperlink ref="A75" r:id="rId13" display="https://www.thebalance.com/a-list-of-short-oil-etfs-1214742" xr:uid="{C848A9F3-803B-41EE-9BF2-18DF2C871D77}"/>
-    <hyperlink ref="A85" r:id="rId14" display="https://www.thebalance.com/what-is-the-dia-diamonds-etf-1214779" xr:uid="{48960D6E-84CC-49A1-9133-89D7B9324347}"/>
-    <hyperlink ref="A104" r:id="rId15" display="https://www.thebalance.com/list-of-dividend-etfs-dividend-funds-1214794" xr:uid="{212AD548-DD46-4D61-AA89-64263AF4065D}"/>
-    <hyperlink ref="A134" r:id="rId16" display="https://www.thebalance.com/region-etfs-and-etns-1215142" xr:uid="{30FBCC66-BC8C-4146-B48C-BC0F44D58A25}"/>
+    <hyperlink ref="A11" r:id="rId1" display="https://www.thebalance.com/list-of-energy-etfs-and-etns-1214760" xr:uid="{11655A6A-FD14-4040-9749-227830CD9695}"/>
+    <hyperlink ref="A21" r:id="rId2" display="https://www.thebalance.com/sdow-a-3x-leveraged-inverse-dow-etf-1215076" xr:uid="{D2112285-2094-4EAA-BE4F-1C95C87AAE55}"/>
+    <hyperlink ref="A23" r:id="rId3" display="https://www.thebalance.com/list-of-leveraged-inverse-etfs-1215227" xr:uid="{9091B37D-4761-448B-BD0A-8BA6049697BA}"/>
+    <hyperlink ref="A35" r:id="rId4" display="https://www.thebalance.com/how-to-invest-in-brazil-with-brazil-etfs-1215127" xr:uid="{7A61D21E-DB11-4DD0-AF99-7D092BB17968}"/>
+    <hyperlink ref="A37" r:id="rId5" display="https://www.thebalance.com/list-of-currency-etfs-and-etns-1215150" xr:uid="{136BEAB0-3B63-402E-90E0-70D6889F7F18}"/>
+    <hyperlink ref="A45" r:id="rId6" display="https://www.thebalance.com/best-cyber-security-etfs-for-2018-4176623" xr:uid="{ABC8736D-C065-4E62-A49B-D9BE59BFAFCD}"/>
+    <hyperlink ref="A49" r:id="rId7" display="https://www.thebalance.com/what-are-futures-and-why-are-they-in-etfs-1214893" xr:uid="{DEC14E35-F05E-43C6-B10B-942E1E443A63}"/>
+    <hyperlink ref="A61" r:id="rId8" display="https://www.thebalance.com/investing-china-etfs-1215166" xr:uid="{9D18CD7A-62E5-4E9C-B26C-E0E802058FB7}"/>
+    <hyperlink ref="A64" r:id="rId9" display="https://www.thebalance.com/learn-the-basics-about-commodity-etfs-1214745" xr:uid="{C7940C82-F295-4443-B03F-6BE2FEFFA78F}"/>
+    <hyperlink ref="A66" r:id="rId10" display="https://www.thebalance.com/gold-etf-what-you-need-to-know-1214748" xr:uid="{7CB792F2-07CC-4BF6-A975-ACDA87540240}"/>
+    <hyperlink ref="A68" r:id="rId11" display="https://www.thebalance.com/how-to-invest-in-oil-without-getting-your-hands-dirty-1214929" xr:uid="{A4BA6A25-556A-4296-941B-A46F8C7D7B8D}"/>
+    <hyperlink ref="A72" r:id="rId12" display="https://www.thebalance.com/list-of-major-oil-etfs-and-etns-1214764" xr:uid="{0130E49E-7202-4A1E-9D26-E5E2E984A789}"/>
+    <hyperlink ref="A76" r:id="rId13" display="https://www.thebalance.com/a-list-of-short-oil-etfs-1214742" xr:uid="{C848A9F3-803B-41EE-9BF2-18DF2C871D77}"/>
+    <hyperlink ref="A86" r:id="rId14" display="https://www.thebalance.com/what-is-the-dia-diamonds-etf-1214779" xr:uid="{48960D6E-84CC-49A1-9133-89D7B9324347}"/>
+    <hyperlink ref="A105" r:id="rId15" display="https://www.thebalance.com/list-of-dividend-etfs-dividend-funds-1214794" xr:uid="{212AD548-DD46-4D61-AA89-64263AF4065D}"/>
+    <hyperlink ref="A135" r:id="rId16" display="https://www.thebalance.com/region-etfs-and-etns-1215142" xr:uid="{30FBCC66-BC8C-4146-B48C-BC0F44D58A25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data split. vix downloaded and reorged. next: insert as platform required.
</commit_message>
<xml_diff>
--- a/0.Data/ETF List.xlsx
+++ b/0.Data/ETF List.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_AD4DC2C4214B839BC62F9C83E64E2CC26AE8DE2C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{DF0B252A-1D14-477A-9CF8-B2F69548A59E}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4DC2C4214B839BC62F9C83E64E2CC26AE8DE2C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BE19B292-DECA-4AA0-B375-A91BE85E8959}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$644</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$647</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -2202,16 +2202,16 @@
   <dimension ref="A1:E647"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D649" sqref="D649"/>
+      <selection activeCell="E317" sqref="E317"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="74.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>596</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>593</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2342,10 +2342,10 @@
         <v>594</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2377,50 +2377,50 @@
         <v>594</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2434,241 +2434,241 @@
         <v>594</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>69</v>
       </c>
@@ -2682,766 +2682,766 @@
         <v>601</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="145" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="146" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="149" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="150" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="151" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="153" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="154" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="155" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="156" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="157" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="158" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="159" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="160" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="161" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="162" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="163" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="164" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="165" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="166" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="168" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="169" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="170" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="171" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="172" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="173" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="174" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="175" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="176" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="177" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="178" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="179" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="181" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="182" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="183" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="184" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="185" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="186" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="187" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="188" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="189" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="190" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="191" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="192" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="194" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="195" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="196" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="197" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="198" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="199" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="200" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="201" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="202" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="203" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="204" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="206" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="207" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="208" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="209" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="210" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="211" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="212" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="213" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="214" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="215" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="216" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="217" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="219" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="220" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="221" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="222" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="223" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="224" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1"/>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>214</v>
       </c>
@@ -3455,365 +3455,365 @@
         <v>594</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="241" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1"/>
     </row>
-    <row r="242" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="243" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="244" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="245" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="246" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="247" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="248" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="249" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="250" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="251" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="252" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="253" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="254" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1"/>
     </row>
-    <row r="255" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="256" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="257" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="258" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="259" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="260" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="261" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="262" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="263" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="264" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="265" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="266" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="1"/>
     </row>
-    <row r="267" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="268" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="269" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="270" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="271" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="272" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="273" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="274" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="275" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="276" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="277" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="278" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1"/>
     </row>
-    <row r="279" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="280" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="281" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="282" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="283" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="284" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="285" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="286" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="287" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="288" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1"/>
     </row>
-    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="291" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="292" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="293" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="294" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="295" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="296" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="297" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="298" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="299" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="300" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="301" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="302" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1"/>
     </row>
-    <row r="303" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="304" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>283</v>
       </c>
@@ -3827,12 +3827,12 @@
         <v>601</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>285</v>
       </c>
@@ -3846,25 +3846,25 @@
         <v>594</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1"/>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>289</v>
       </c>
@@ -3878,32 +3878,32 @@
         <v>603</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>295</v>
       </c>
@@ -3917,219 +3917,219 @@
         <v>594</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="1"/>
     </row>
-    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="337" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="338" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="339" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="340" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="1"/>
     </row>
-    <row r="341" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="342" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="343" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="344" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="345" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="346" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="347" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="348" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="349" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="350" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="351" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="352" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="1"/>
     </row>
-    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="355" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="362" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="1"/>
     </row>
-    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
         <v>336</v>
       </c>
@@ -4143,889 +4143,889 @@
         <v>601</v>
       </c>
     </row>
-    <row r="369" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="370" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="371" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="372" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="373" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="374" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="375" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="376" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="377" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="378" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" s="1"/>
     </row>
-    <row r="379" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="380" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="381" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="382" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="383" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="384" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="385" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="386" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="387" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="388" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="389" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="390" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="1"/>
     </row>
-    <row r="391" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="392" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="393" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="394" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="395" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="396" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="397" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="398" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="399" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="400" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="401" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="402" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" s="1"/>
     </row>
-    <row r="403" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="404" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="405" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="406" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="407" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="408" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="409" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="410" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="411" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="412" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="413" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A413" s="1"/>
     </row>
-    <row r="414" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="415" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="416" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="417" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="418" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="419" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="420" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="421" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="422" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="423" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="424" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="425" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A425" s="1"/>
     </row>
-    <row r="426" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="427" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="428" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="429" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="430" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="431" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="432" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="433" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="434" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="435" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="436" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="437" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="438" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438" s="1"/>
     </row>
-    <row r="439" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="440" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="441" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="442" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="443" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="444" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="445" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="446" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="447" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="448" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="449" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="450" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="451" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="452" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A452" s="1"/>
     </row>
-    <row r="453" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="454" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="455" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="456" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="457" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="458" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="459" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="460" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="461" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="462" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="463" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="464" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="465" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="466" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="467" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A467" s="1"/>
     </row>
-    <row r="468" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="469" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="470" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="471" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="472" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="473" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="474" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="475" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A475" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="476" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A476" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="477" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="478" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="479" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="480" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="481" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" s="1"/>
     </row>
-    <row r="482" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="483" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="484" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="485" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="486" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A486" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="487" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A487" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="488" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A488" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="489" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A489" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="490" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A490" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="491" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A491" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="492" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="493" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="494" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A494" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="495" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A495" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="496" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496" s="1"/>
     </row>
-    <row r="497" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="498" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A498" s="1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="499" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A499" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="500" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="501" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A501" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="502" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A502" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="503" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A503" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="504" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A504" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="505" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A505" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="506" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A506" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="507" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A507" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="508" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A508" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="509" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A509" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="510" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A510" s="1"/>
     </row>
-    <row r="511" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="512" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A512" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="513" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A513" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="514" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A514" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="515" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A515" s="1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="516" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A516" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="517" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A517" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="518" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A518" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="519" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A519" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="520" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A520" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="521" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A521" s="1" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="522" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A522" s="1" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="523" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A523" s="1" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="524" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A524" s="1"/>
     </row>
-    <row r="525" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A525" s="1" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="526" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A526" s="1" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="527" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A527" s="1" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="528" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A528" s="1" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="529" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A529" s="1" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="530" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A530" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="531" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A531" s="1" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="532" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A532" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="533" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A533" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="534" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A534" s="1" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="535" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A535" s="1"/>
     </row>
-    <row r="536" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A536" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="537" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A537" s="1" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="538" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A538" s="1" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="539" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="540" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A540" s="1" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="541" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A541" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="542" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A542" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="543" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A543" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="544" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A544" s="1" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="545" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A545" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="546" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A546" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="547" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A547" s="1"/>
     </row>
-    <row r="548" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A548" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="549" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A549" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="550" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A550" s="1" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="551" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A551" s="1" t="s">
         <v>505</v>
       </c>
@@ -5039,22 +5039,22 @@
         <v>594</v>
       </c>
     </row>
-    <row r="552" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A552" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="553" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A553" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="554" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A554" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A555" s="1" t="s">
         <v>509</v>
       </c>
@@ -5068,201 +5068,201 @@
         <v>602</v>
       </c>
     </row>
-    <row r="556" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A556" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="557" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A557" s="1" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="558" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A558" s="1" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="559" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A559" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="560" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A560" s="1" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="561" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A561" s="1"/>
     </row>
-    <row r="562" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A562" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="563" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A563" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="564" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A564" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="565" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A565" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="566" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A566" s="1" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="567" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A567" s="1" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="568" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A568" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="569" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A569" s="1" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="570" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A570" s="1" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="571" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A571" s="1" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="572" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A572" s="1" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="573" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A573" s="1" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="574" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A574" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="575" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A575" s="1" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="576" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A576" s="1"/>
     </row>
-    <row r="577" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A577" s="1" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="578" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A578" s="1" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="579" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A579" s="1" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="580" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A580" s="1" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="581" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A581" s="1" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="582" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A582" s="1" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="583" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A583" s="1" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="584" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A584" s="1" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="585" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A585" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="586" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="586" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A586" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="587" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A587" s="1" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="588" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A588" s="1" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="589" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A589" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="590" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A590" s="1" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="591" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A591" s="1"/>
     </row>
-    <row r="592" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A592" s="1" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="593" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A593" s="1" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="594" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A594" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="595" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A595" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="596" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A596" s="1" t="s">
         <v>547</v>
       </c>
@@ -5276,55 +5276,55 @@
         <v>601</v>
       </c>
     </row>
-    <row r="597" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A597" s="1" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="598" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A598" s="1" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="599" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A599" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="600" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A600" s="1" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="601" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A601" s="1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="602" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A602" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="603" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A603" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="604" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A604" s="1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="605" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A605" s="1"/>
     </row>
-    <row r="606" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A606" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="607" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A607" s="1" t="s">
         <v>557</v>
       </c>
@@ -5338,120 +5338,120 @@
         <v>594</v>
       </c>
     </row>
-    <row r="608" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A608" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="609" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A609" s="1" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="610" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A610" s="1" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="611" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A611" s="1" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="612" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A612" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="613" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A613" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="614" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A614" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="615" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A615" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="616" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A616" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="617" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A617" s="1" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="618" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A618" s="1" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="619" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A619" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="620" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A620" s="1"/>
     </row>
-    <row r="621" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A621" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="622" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A622" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="623" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A623" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="624" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A624" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="625" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A625" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="626" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A626" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="627" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="627" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A627" s="1" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="628" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A628" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="629" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A629" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="630" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A630" s="1" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="631" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A631" s="1" t="s">
         <v>580</v>
       </c>
@@ -5465,70 +5465,70 @@
         <v>594</v>
       </c>
     </row>
-    <row r="632" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="632" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A632" s="1" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="633" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="633" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A633" s="1" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="634" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A634" s="1" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="635" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A635" s="1"/>
     </row>
-    <row r="636" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A636" s="1" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="637" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A637" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="638" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A638" s="1" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="639" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A639" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="640" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A640" s="1" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="641" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="641" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A641" s="1" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="642" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="642" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A642" s="1" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="643" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="643" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A643" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="644" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="644" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A644" s="1" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="645" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="645" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A645" s="1" t="s">
         <v>604</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="646" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="646" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A646" s="1" t="s">
         <v>605</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="647" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="647" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A647" s="1" t="s">
         <v>606</v>
       </c>
@@ -5553,7 +5553,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E644" xr:uid="{021B84DF-B46C-42BE-8F95-15AC20779B95}">
+  <autoFilter ref="E1:E647" xr:uid="{2B38BA4A-182C-4BCD-BEF5-5EB6FDE311D7}">
     <filterColumn colId="0">
       <filters>
         <filter val="Y"/>

</xml_diff>